<commit_message>
Se agregan las 4 semanas al Cronograma con sus respectivas fechas
</commit_message>
<xml_diff>
--- a/Cronograma_de_Actividades_UdeA.xlsx
+++ b/Cronograma_de_Actividades_UdeA.xlsx
@@ -8,12 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PERSONAL\Desktop\Universidad de Antioquia\UdeA 2023-1\Cronograma UdeA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3BD1A46-604F-431C-90BC-5D5F6FB37A72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D85260B7-0A62-4AF5-BF5C-87BF3095C0B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{67A782D1-A15B-4321-AF5D-AE38C04A4B78}"/>
   </bookViews>
   <sheets>
-    <sheet name="13-19 de febrero" sheetId="1" r:id="rId1"/>
+    <sheet name="13-19 de Febrero" sheetId="1" r:id="rId1"/>
+    <sheet name="20-26 de Febrero" sheetId="2" r:id="rId2"/>
+    <sheet name="27 de Febrero - 5 de Marzo" sheetId="4" r:id="rId3"/>
+    <sheet name="6-12 de Marzo" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,37 +39,128 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
   <si>
     <t>CRONOGRAMA UDEA</t>
   </si>
   <si>
-    <t>Lunes</t>
-  </si>
-  <si>
-    <t>Martes</t>
-  </si>
-  <si>
-    <t>Miercoles</t>
-  </si>
-  <si>
-    <t>Jueves</t>
-  </si>
-  <si>
-    <t>Viernes</t>
-  </si>
-  <si>
-    <t>Sabado</t>
-  </si>
-  <si>
-    <t>Domingo</t>
+    <t>Lunes
+13 de Febrero</t>
+  </si>
+  <si>
+    <t>Martes
+14 de Febrero</t>
+  </si>
+  <si>
+    <t>Miercoles
+15 de Febrero</t>
+  </si>
+  <si>
+    <t>Jueves
+16 de Febrero</t>
+  </si>
+  <si>
+    <t>Viernes
+17 de Febrero</t>
+  </si>
+  <si>
+    <t>Sabado
+18 de Febrero</t>
+  </si>
+  <si>
+    <t>Domingo
+19 de Febrero</t>
+  </si>
+  <si>
+    <t>Lunes
+20 de Febrero</t>
+  </si>
+  <si>
+    <t>Martes
+21 de Febrero</t>
+  </si>
+  <si>
+    <t>Miercoles
+22 de Febrero</t>
+  </si>
+  <si>
+    <t>Jueves
+23 de Febrero</t>
+  </si>
+  <si>
+    <t>Viernes
+24 de Febrero</t>
+  </si>
+  <si>
+    <t>Sabado
+25 de Febrero</t>
+  </si>
+  <si>
+    <t>Domingo
+26 de Febrero</t>
+  </si>
+  <si>
+    <t>Lunes
+27 de Febrero</t>
+  </si>
+  <si>
+    <t>Martes
+28 de Febrero</t>
+  </si>
+  <si>
+    <t>Miercoles
+1 de Marzo</t>
+  </si>
+  <si>
+    <t>Jueves
+2 de Marzo</t>
+  </si>
+  <si>
+    <t>Viernes
+3 de Marzo</t>
+  </si>
+  <si>
+    <t>Sabado
+4 de Marzo</t>
+  </si>
+  <si>
+    <t>Domingo
+5 de Marzo</t>
+  </si>
+  <si>
+    <t>Lunes
+6 de Marzo</t>
+  </si>
+  <si>
+    <t>Martes
+7 de Marzo</t>
+  </si>
+  <si>
+    <t>Miercoles
+8 de Marzo</t>
+  </si>
+  <si>
+    <t>Jueves
+9 de Marzo</t>
+  </si>
+  <si>
+    <t>Viernes
+10 de Marzo</t>
+  </si>
+  <si>
+    <t>Sabado
+11 de Marzo</t>
+  </si>
+  <si>
+    <t>Domingo
+12 de Marzo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -86,6 +180,14 @@
       <b/>
       <sz val="18"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -117,10 +219,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -437,27 +545,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9BE88BC-B312-4FC5-B9C4-7BC7FEB3A553}">
-  <dimension ref="B1:J3"/>
+  <dimension ref="B2:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="B2" sqref="B2:H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="8" width="12.44140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B1" s="2" t="s">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-    </row>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
@@ -468,31 +570,233 @@
       <c r="J2" s="1"/>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B3" t="s">
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+    </row>
+    <row r="4" spans="2:10" s="4" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H4" s="3" t="s">
         <v>7</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B1:H2"/>
+    <mergeCell ref="B2:H3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A9DB7A8-096E-45F4-9032-968A820EB1B3}">
+  <dimension ref="B2:H4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="8" width="12.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+    </row>
+    <row r="4" spans="2:8" s="4" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:H3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{996034FA-BD3D-4306-9E3E-A7338EEA49DE}">
+  <dimension ref="B2:H4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="8" width="12.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+    </row>
+    <row r="4" spans="2:8" s="4" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:H3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFE6A262-896D-4162-977E-4D5EA36017DD}">
+  <dimension ref="B2:H4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="8" width="12.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+    </row>
+    <row r="4" spans="2:8" s="4" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:H3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Todo fue un Caos y me estresé
</commit_message>
<xml_diff>
--- a/Cronograma_de_Actividades_UdeA.xlsx
+++ b/Cronograma_de_Actividades_UdeA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PERSONAL\Desktop\Universidad de Antioquia\UdeA 2023-1\Cronograma UdeA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D85260B7-0A62-4AF5-BF5C-87BF3095C0B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3073D450-3339-4065-A6E0-019C9E06CD10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{67A782D1-A15B-4321-AF5D-AE38C04A4B78}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="55">
   <si>
     <t>CRONOGRAMA UDEA</t>
   </si>
@@ -154,13 +154,99 @@
   <si>
     <t>Domingo
 12 de Marzo</t>
+  </si>
+  <si>
+    <t>6-7</t>
+  </si>
+  <si>
+    <t>7-8</t>
+  </si>
+  <si>
+    <t>8-9</t>
+  </si>
+  <si>
+    <t>10-11</t>
+  </si>
+  <si>
+    <t>11-12</t>
+  </si>
+  <si>
+    <t>12-13</t>
+  </si>
+  <si>
+    <t>13-14</t>
+  </si>
+  <si>
+    <t>14-15</t>
+  </si>
+  <si>
+    <t>16-17</t>
+  </si>
+  <si>
+    <t>17-18</t>
+  </si>
+  <si>
+    <t>15-16</t>
+  </si>
+  <si>
+    <t>18-19</t>
+  </si>
+  <si>
+    <t>19-20</t>
+  </si>
+  <si>
+    <t>20-21</t>
+  </si>
+  <si>
+    <t>21-22</t>
+  </si>
+  <si>
+    <t>22-23</t>
+  </si>
+  <si>
+    <t>23-24</t>
+  </si>
+  <si>
+    <t>Hora-Día</t>
+  </si>
+  <si>
+    <t>5-6</t>
+  </si>
+  <si>
+    <t>TEORIA
+INFORMATICA II</t>
+  </si>
+  <si>
+    <t>INGLES VI</t>
+  </si>
+  <si>
+    <t>LABORATORIO
+CIRCUITOS
+ELECTRICOS I</t>
+  </si>
+  <si>
+    <t>TEORIA
+CIRCUITOS
+ELECTRICOS I</t>
+  </si>
+  <si>
+    <t>TEORIA DE LA
+INFORMACIÓN</t>
+  </si>
+  <si>
+    <t>LABORATORIO
+INFORMATICA II</t>
+  </si>
+  <si>
+    <t>REFERENCIACION
+GEOGRAFICA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -192,8 +278,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF00FF00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -206,8 +306,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -215,21 +321,389 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -237,6 +711,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF00FF00"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -545,10 +1024,343 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9BE88BC-B312-4FC5-B9C4-7BC7FEB3A553}">
-  <dimension ref="B2:J4"/>
+  <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:H3"/>
+      <selection activeCell="K11" sqref="K11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="3" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="1"/>
+    </row>
+    <row r="3" spans="2:10" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="22"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="24"/>
+    </row>
+    <row r="4" spans="2:10" s="3" customFormat="1" ht="44.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="H4" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="I4" s="21" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="43" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" s="25"/>
+      <c r="D5" s="47"/>
+      <c r="F5" s="47" t="s">
+        <v>49</v>
+      </c>
+      <c r="G5" s="12"/>
+      <c r="H5" s="25"/>
+      <c r="I5" s="27"/>
+    </row>
+    <row r="6" spans="2:10" ht="44.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="44" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="15"/>
+      <c r="D6" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="E6" s="50" t="s">
+        <v>50</v>
+      </c>
+      <c r="F6" s="48"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="16"/>
+    </row>
+    <row r="7" spans="2:10" ht="15.6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="45" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="12"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="51"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="14"/>
+    </row>
+    <row r="8" spans="2:10" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="44" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="15"/>
+      <c r="D8" s="35" t="s">
+        <v>48</v>
+      </c>
+      <c r="E8" s="37"/>
+      <c r="F8" s="33" t="s">
+        <v>48</v>
+      </c>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="16"/>
+    </row>
+    <row r="9" spans="2:10" ht="23.4" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="45" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="12"/>
+      <c r="D9" s="41"/>
+      <c r="E9" s="38" t="s">
+        <v>51</v>
+      </c>
+      <c r="F9" s="49"/>
+      <c r="G9" s="38" t="s">
+        <v>51</v>
+      </c>
+      <c r="H9" s="12"/>
+      <c r="I9" s="14"/>
+    </row>
+    <row r="10" spans="2:10" ht="23.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="29"/>
+      <c r="F10" s="39"/>
+      <c r="G10" s="40"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="16"/>
+    </row>
+    <row r="11" spans="2:10" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="45" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="25"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="14"/>
+    </row>
+    <row r="12" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="44" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
+      <c r="I12" s="16"/>
+    </row>
+    <row r="13" spans="2:10" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="45" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="30" t="s">
+        <v>54</v>
+      </c>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="14"/>
+    </row>
+    <row r="14" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="31"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="15"/>
+      <c r="I14" s="16"/>
+    </row>
+    <row r="15" spans="2:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="45" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" s="32"/>
+      <c r="D15" s="35" t="s">
+        <v>52</v>
+      </c>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="33" t="s">
+        <v>52</v>
+      </c>
+      <c r="H15" s="12"/>
+      <c r="I15" s="14"/>
+    </row>
+    <row r="16" spans="2:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="44" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" s="42"/>
+      <c r="D16" s="36"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="34"/>
+      <c r="H16" s="15"/>
+      <c r="I16" s="16"/>
+    </row>
+    <row r="17" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" s="12"/>
+      <c r="D17" s="38" t="s">
+        <v>53</v>
+      </c>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="14"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B18" s="44" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" s="15"/>
+      <c r="D18" s="40"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="15"/>
+      <c r="I18" s="16"/>
+    </row>
+    <row r="19" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B19" s="45" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" s="12"/>
+      <c r="D19" s="29"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="14"/>
+    </row>
+    <row r="20" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="44" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" s="15"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="15"/>
+      <c r="H20" s="15"/>
+      <c r="I20" s="16"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B21" s="45" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21" s="12"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="14"/>
+    </row>
+    <row r="22" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B22" s="46" t="s">
+        <v>45</v>
+      </c>
+      <c r="C22" s="17"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="17"/>
+      <c r="G22" s="17"/>
+      <c r="H22" s="17"/>
+      <c r="I22" s="18"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23" s="4"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24" s="4"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A25" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="D17:D19"/>
+    <mergeCell ref="G15:G16"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="C13:C15"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="B2:I3"/>
+  </mergeCells>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="B11" twoDigitTextYear="1"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A9DB7A8-096E-45F4-9032-968A820EB1B3}">
+  <dimension ref="A2:H22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -556,49 +1368,140 @@
     <col min="2" max="8" width="12.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B2" s="2" t="s">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-    </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-    </row>
-    <row r="4" spans="2:10" s="4" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B4" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>7</v>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+    </row>
+    <row r="4" spans="1:8" s="3" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" s="5" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -606,16 +1509,18 @@
     <mergeCell ref="B2:H3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="A11" twoDigitTextYear="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A9DB7A8-096E-45F4-9032-968A820EB1B3}">
-  <dimension ref="B2:H4"/>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{996034FA-BD3D-4306-9E3E-A7338EEA49DE}">
+  <dimension ref="A2:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -623,47 +1528,140 @@
     <col min="2" max="8" width="12.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B2" s="2" t="s">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-    </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-    </row>
-    <row r="4" spans="2:8" s="4" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>14</v>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+    </row>
+    <row r="4" spans="1:8" s="3" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" s="5" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -671,15 +1669,18 @@
     <mergeCell ref="B2:H3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="A11" twoDigitTextYear="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{996034FA-BD3D-4306-9E3E-A7338EEA49DE}">
-  <dimension ref="B2:H4"/>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFE6A262-896D-4162-977E-4D5EA36017DD}">
+  <dimension ref="A2:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -687,47 +1688,140 @@
     <col min="2" max="8" width="12.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B2" s="2" t="s">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-    </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-    </row>
-    <row r="4" spans="2:8" s="4" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B4" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>21</v>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+    </row>
+    <row r="4" spans="1:8" s="3" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" s="5" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -735,69 +1829,8 @@
     <mergeCell ref="B2:H3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFE6A262-896D-4162-977E-4D5EA36017DD}">
-  <dimension ref="B2:H4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="2" max="8" width="12.44140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-    </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-    </row>
-    <row r="4" spans="2:8" s="4" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B4" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B2:H3"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="A11" twoDigitTextYear="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>